<commit_message>
Refactorizacion de los métodos que extienden de tarjeta
</commit_message>
<xml_diff>
--- a/Practica5Refactorizado/src/main/resources/metricas.xlsx
+++ b/Practica5Refactorizado/src/main/resources/metricas.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\My_Projects\eclipse-workspace\Practica5Refactorizado\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{493FAB2D-E9A5-4BFA-AFD4-31CAB2A758C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EB6FA396-8606-4A57-AB4C-DE3C02E09070}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13308" yWindow="1572" windowWidth="17280" windowHeight="8964" xr2:uid="{842FBD3A-5DF2-4DD6-BAAE-EBFB7E3BCC80}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="17310" windowHeight="12435" xr2:uid="{842FBD3A-5DF2-4DD6-BAAE-EBFB7E3BCC80}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -94,8 +90,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,9 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,15 +449,15 @@
   <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>11</v>
       </c>
@@ -471,7 +477,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -481,8 +487,9 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -493,7 +500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -504,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -515,7 +522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -526,7 +533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -537,7 +544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -548,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -559,33 +566,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -602,7 +609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -613,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -621,7 +628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -632,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>4</v>
       </c>
@@ -643,7 +650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>5</v>
       </c>
@@ -651,7 +658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>6</v>
       </c>
@@ -659,7 +666,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>7</v>
       </c>
@@ -667,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>8</v>
       </c>
@@ -677,5 +684,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>